<commit_message>
fix some requirement issue.
</commit_message>
<xml_diff>
--- a/ConstructionCalculator.Business.Test/TestResource/BusinessFeature.xlsx
+++ b/ConstructionCalculator.Business.Test/TestResource/BusinessFeature.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\einst\Documents\GitHub\ConstructionCalculator\ConstructionCalculator.Business.Test\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Construction Calculator\ImportData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>业态特征ID</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -62,378 +62,210 @@
     <t>价值因子</t>
   </si>
   <si>
-    <t>101</t>
-  </si>
-  <si>
     <t>室内停车场</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>102</t>
-  </si>
-  <si>
     <t>室外机械立体停车库</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>103</t>
-  </si>
-  <si>
     <t>室内汽车销售</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>104</t>
-  </si>
-  <si>
     <t>室内汽车修理</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>105</t>
-  </si>
-  <si>
     <t>地下停车库</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>201</t>
-  </si>
-  <si>
     <t>别墅、自建房</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>202</t>
-  </si>
-  <si>
     <t>多层单元住宅</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>203</t>
-  </si>
-  <si>
     <t>高层住宅</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>301</t>
-  </si>
-  <si>
     <t>公寓</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>302</t>
-  </si>
-  <si>
     <t>小型宾馆</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>303</t>
-  </si>
-  <si>
     <t>高档型宾馆</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>501</t>
-  </si>
-  <si>
     <t>学生宿舍</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>502</t>
-  </si>
-  <si>
     <t>职工宿舍</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>601</t>
-  </si>
-  <si>
     <t>歌舞类</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>602</t>
-  </si>
-  <si>
     <t>放映类</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>603</t>
-  </si>
-  <si>
     <t>室内休闲游艺类</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>604</t>
-  </si>
-  <si>
     <t>室内健身</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>605</t>
-  </si>
-  <si>
     <t>室内运动场</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>606</t>
-  </si>
-  <si>
     <t>室内洗浴场所类</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>801</t>
-  </si>
-  <si>
     <t>商铺</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>802</t>
-  </si>
-  <si>
     <t>成组布置、连片经营市场</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>803</t>
-  </si>
-  <si>
     <t>购物中心</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>901</t>
-  </si>
-  <si>
     <t>候车楼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>902</t>
-  </si>
-  <si>
     <t>侯船楼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>903</t>
-  </si>
-  <si>
     <t>候机楼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1001</t>
-  </si>
-  <si>
     <t>农贸市场</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1101</t>
-  </si>
-  <si>
     <t>餐馆</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1102</t>
-  </si>
-  <si>
     <t>食堂</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1201</t>
-  </si>
-  <si>
     <t>图书馆</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1202</t>
-  </si>
-  <si>
     <t>展览馆</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1203</t>
-  </si>
-  <si>
     <t>博物馆</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1204</t>
-  </si>
-  <si>
     <t>科技馆</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1301</t>
-  </si>
-  <si>
     <t>教学楼、培训场所</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1401</t>
-  </si>
-  <si>
     <t>托儿所、幼儿园</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1501</t>
-  </si>
-  <si>
     <t>寺庙、教堂等</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1601</t>
-  </si>
-  <si>
     <t>监狱和拘留所</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1701</t>
-  </si>
-  <si>
     <t>门诊楼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1702</t>
-  </si>
-  <si>
     <t>住院楼</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1703</t>
-  </si>
-  <si>
     <t>养老院</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1704</t>
-  </si>
-  <si>
     <t>福利院</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1801</t>
-  </si>
-  <si>
     <t>生产加工丁、戊类产品</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>1901</t>
-  </si>
-  <si>
     <t>生产加工丙类固体</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2001</t>
-  </si>
-  <si>
     <t>甲乙类固体</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2002</t>
-  </si>
-  <si>
     <t>甲乙类气体</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2003</t>
-  </si>
-  <si>
     <t>甲乙类液体</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2004</t>
-  </si>
-  <si>
     <t>丙类液体</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2101</t>
-  </si>
-  <si>
     <t>丙类固体生产过程中存在粉尘</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2201</t>
-  </si>
-  <si>
     <t>存储丁、戊类物品</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2301</t>
-  </si>
-  <si>
     <t>存储丙类固体</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2401</t>
-  </si>
-  <si>
-    <t>2402</t>
-  </si>
-  <si>
-    <t>2403</t>
-  </si>
-  <si>
-    <t>2404</t>
-  </si>
-  <si>
-    <t>2501</t>
-  </si>
-  <si>
     <t>丙类固体存储环境存在可燃粉尘</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2601</t>
-  </si>
-  <si>
     <t>冷链物流</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2701</t>
-  </si>
-  <si>
     <t>多合一场所</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -442,17 +274,21 @@
   </si>
   <si>
     <t>城市综合体</t>
+  </si>
+  <si>
+    <t>废弃场所</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -484,6 +320,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -493,7 +336,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -516,11 +359,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -531,9 +385,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -543,9 +394,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -857,16 +730,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -900,12 +776,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="25.5">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -916,13 +792,13 @@
       <c r="E2" s="1">
         <v>1500</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>0.89</v>
       </c>
-      <c r="G2" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H2" s="5">
+      <c r="G2" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="4">
         <v>0.1</v>
       </c>
       <c r="I2" s="1">
@@ -931,16 +807,16 @@
       <c r="J2" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>0.17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="38.25">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
+    <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -951,13 +827,13 @@
       <c r="E3" s="1">
         <v>1500</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.89</v>
       </c>
-      <c r="G3" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H3" s="5">
+      <c r="G3" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="4">
         <v>0.1</v>
       </c>
       <c r="I3" s="1">
@@ -966,16 +842,16 @@
       <c r="J3" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>0.26</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="25.5">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -986,13 +862,13 @@
       <c r="E4" s="1">
         <v>1500</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.89</v>
       </c>
-      <c r="G4" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="G4" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H4" s="4">
         <v>0.1</v>
       </c>
       <c r="I4" s="1">
@@ -1001,16 +877,16 @@
       <c r="J4" s="3">
         <v>0.75</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="25.5">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
+    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -1021,13 +897,13 @@
       <c r="E5" s="1">
         <v>1500</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.89</v>
       </c>
-      <c r="G5" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="G5" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="4">
         <v>0.1</v>
       </c>
       <c r="I5" s="1">
@@ -1036,16 +912,16 @@
       <c r="J5" s="3">
         <v>0.01</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>0.12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="25.5">
-      <c r="A6" s="4" t="s">
-        <v>19</v>
+    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1056,13 +932,13 @@
       <c r="E6" s="1">
         <v>1500</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.89</v>
       </c>
-      <c r="G6" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H6" s="5">
+      <c r="G6" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="4">
         <v>0.1</v>
       </c>
       <c r="I6" s="1">
@@ -1071,16 +947,16 @@
       <c r="J6" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="25.5">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
+    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>201</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -1091,13 +967,13 @@
       <c r="E7" s="1">
         <v>600</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>0.89</v>
       </c>
-      <c r="G7" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H7" s="5">
+      <c r="G7" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="4">
         <v>0.1</v>
       </c>
       <c r="I7" s="1">
@@ -1106,16 +982,16 @@
       <c r="J7" s="3">
         <v>0.04</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="25.5">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
+    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>202</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -1126,13 +1002,13 @@
       <c r="E8" s="1">
         <v>600</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>0.89</v>
       </c>
-      <c r="G8" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="G8" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="4">
         <v>0.1</v>
       </c>
       <c r="I8" s="1">
@@ -1141,16 +1017,16 @@
       <c r="J8" s="3">
         <v>0.03</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>203</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -1161,13 +1037,13 @@
       <c r="E9" s="1">
         <v>600</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0.89</v>
       </c>
-      <c r="G9" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H9" s="5">
+      <c r="G9" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="4">
         <v>0.1</v>
       </c>
       <c r="I9" s="1">
@@ -1176,16 +1052,16 @@
       <c r="J9" s="3">
         <v>0.03</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="4" t="s">
-        <v>27</v>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>301</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2">
         <v>3</v>
@@ -1196,13 +1072,13 @@
       <c r="E10" s="1">
         <v>600</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>0.89</v>
       </c>
-      <c r="G10" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="G10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="4">
         <v>0.2</v>
       </c>
       <c r="I10" s="1">
@@ -1211,16 +1087,16 @@
       <c r="J10" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="4">
         <v>0.08</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="4" t="s">
-        <v>29</v>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>302</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
@@ -1231,13 +1107,13 @@
       <c r="E11" s="1">
         <v>600</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>0.89</v>
       </c>
-      <c r="G11" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H11" s="5">
+      <c r="G11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="4">
         <v>0.2</v>
       </c>
       <c r="I11" s="1">
@@ -1246,16 +1122,16 @@
       <c r="J11" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="25.5">
-      <c r="A12" s="4" t="s">
-        <v>31</v>
+    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>303</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
@@ -1266,13 +1142,13 @@
       <c r="E12" s="1">
         <v>600</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>0.89</v>
       </c>
-      <c r="G12" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H12" s="5">
+      <c r="G12" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="4">
         <v>0.2</v>
       </c>
       <c r="I12" s="1">
@@ -1281,16 +1157,16 @@
       <c r="J12" s="3">
         <v>0.05</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="25.5">
-      <c r="A13" s="4">
+    <row r="13" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
         <v>401</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
@@ -1301,13 +1177,13 @@
       <c r="E13" s="1">
         <v>600</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>0.89</v>
       </c>
-      <c r="G13" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H13" s="5">
+      <c r="G13" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="4">
         <v>0.2</v>
       </c>
       <c r="I13" s="1">
@@ -1316,16 +1192,16 @@
       <c r="J13" s="3">
         <v>0.25</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="4">
         <v>0.12</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="4" t="s">
-        <v>33</v>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>501</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2">
         <v>5</v>
@@ -1336,13 +1212,13 @@
       <c r="E14" s="1">
         <v>600</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G14" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H14" s="5">
+      <c r="G14" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H14" s="4">
         <v>0.1</v>
       </c>
       <c r="I14" s="1">
@@ -1351,16 +1227,16 @@
       <c r="J14" s="3">
         <v>0.25</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="4">
         <v>0.06</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="4" t="s">
-        <v>35</v>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>502</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2">
         <v>5</v>
@@ -1371,13 +1247,13 @@
       <c r="E15" s="1">
         <v>600</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G15" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H15" s="5">
+      <c r="G15" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="4">
         <v>0.1</v>
       </c>
       <c r="I15" s="1">
@@ -1386,16 +1262,16 @@
       <c r="J15" s="3">
         <v>0.16</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="4">
         <v>0.06</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="4" t="s">
-        <v>37</v>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>601</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2">
         <v>6</v>
@@ -1406,13 +1282,13 @@
       <c r="E16" s="1">
         <v>1000</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>1.23</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>0.35</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <v>0.3</v>
       </c>
       <c r="I16" s="1">
@@ -1421,16 +1297,16 @@
       <c r="J16" s="3">
         <v>0.5</v>
       </c>
-      <c r="K16" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="4" t="s">
-        <v>39</v>
+      <c r="K16" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>602</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2">
         <v>6</v>
@@ -1441,13 +1317,13 @@
       <c r="E17" s="1">
         <v>1000</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>1.23</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>0.35</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <v>0.3</v>
       </c>
       <c r="I17" s="1">
@@ -1456,16 +1332,16 @@
       <c r="J17" s="3">
         <v>1</v>
       </c>
-      <c r="K17" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="25.5">
-      <c r="A18" s="4" t="s">
-        <v>41</v>
+      <c r="K17" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>603</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2">
         <v>6</v>
@@ -1476,13 +1352,13 @@
       <c r="E18" s="1">
         <v>800</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G18" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H18" s="5">
+      <c r="G18" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H18" s="4">
         <v>0.2</v>
       </c>
       <c r="I18" s="1">
@@ -1491,16 +1367,16 @@
       <c r="J18" s="3">
         <v>0.1</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="4">
         <v>0.18</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="4" t="s">
-        <v>43</v>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>604</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2">
         <v>6</v>
@@ -1511,13 +1387,13 @@
       <c r="E19" s="1">
         <v>600</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G19" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H19" s="5">
+      <c r="G19" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="4">
         <v>0.2</v>
       </c>
       <c r="I19" s="1">
@@ -1526,16 +1402,16 @@
       <c r="J19" s="3">
         <v>0.1</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="4">
         <v>0.12</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="25.5">
-      <c r="A20" s="4" t="s">
-        <v>45</v>
+    <row r="20" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
+        <v>605</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2">
         <v>6</v>
@@ -1546,31 +1422,31 @@
       <c r="E20" s="1">
         <v>200</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>0.89</v>
       </c>
-      <c r="G20" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H20" s="5">
+      <c r="G20" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H20" s="4">
         <v>0.2</v>
       </c>
       <c r="I20" s="1">
         <v>1.7</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>0.05</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20" s="4">
         <v>0.04</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="25.5">
-      <c r="A21" s="4" t="s">
-        <v>47</v>
+    <row r="21" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <v>606</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2">
         <v>6</v>
@@ -1581,13 +1457,13 @@
       <c r="E21" s="1">
         <v>600</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G21" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H21" s="5">
+      <c r="G21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H21" s="4">
         <v>0.2</v>
       </c>
       <c r="I21" s="1">
@@ -1596,16 +1472,16 @@
       <c r="J21" s="3">
         <v>0.1</v>
       </c>
-      <c r="K21" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="25.5">
-      <c r="A22" s="4">
+      <c r="K21" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
         <v>701</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C22" s="2">
         <v>7</v>
@@ -1631,16 +1507,16 @@
       <c r="J22" s="3">
         <v>0.5</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="4" t="s">
-        <v>49</v>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>801</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2">
         <v>8</v>
@@ -1666,16 +1542,16 @@
       <c r="J23" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="38.25">
-      <c r="A24" s="4" t="s">
-        <v>51</v>
+    <row r="24" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>802</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2">
         <v>8</v>
@@ -1701,16 +1577,16 @@
       <c r="J24" s="3">
         <v>0.15</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="4" t="s">
-        <v>53</v>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>803</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2">
         <v>8</v>
@@ -1736,16 +1612,16 @@
       <c r="J25" s="3">
         <v>0.5</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="4" t="s">
-        <v>55</v>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>901</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2">
         <v>9</v>
@@ -1771,16 +1647,16 @@
       <c r="J26" s="3">
         <v>0.91</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K26" s="4">
         <v>0.09</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="4" t="s">
-        <v>57</v>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>902</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C27" s="2">
         <v>9</v>
@@ -1806,16 +1682,16 @@
       <c r="J27" s="3">
         <v>0.91</v>
       </c>
-      <c r="K27" s="5">
+      <c r="K27" s="4">
         <v>0.09</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="4" t="s">
-        <v>59</v>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>903</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="C28" s="2">
         <v>9</v>
@@ -1841,16 +1717,16 @@
       <c r="J28" s="3">
         <v>0.91</v>
       </c>
-      <c r="K28" s="5">
+      <c r="K28" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="4" t="s">
-        <v>61</v>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>1001</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C29" s="2">
         <v>10</v>
@@ -1876,16 +1752,16 @@
       <c r="J29" s="3">
         <v>0.5</v>
       </c>
-      <c r="K29" s="5">
+      <c r="K29" s="4">
         <v>0.09</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="4" t="s">
-        <v>63</v>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>1101</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C30" s="2">
         <v>11</v>
@@ -1911,16 +1787,16 @@
       <c r="J30" s="3">
         <v>0.77</v>
       </c>
-      <c r="K30" s="5">
+      <c r="K30" s="4">
         <v>0.12</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="4" t="s">
-        <v>65</v>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>1102</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2">
         <v>11</v>
@@ -1946,16 +1822,16 @@
       <c r="J31" s="3">
         <v>1</v>
       </c>
-      <c r="K31" s="5">
+      <c r="K31" s="4">
         <v>0.08</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="4" t="s">
-        <v>67</v>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
+        <v>1201</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C32" s="2">
         <v>12</v>
@@ -1981,16 +1857,16 @@
       <c r="J32" s="3">
         <v>0.1</v>
       </c>
-      <c r="K32" s="5">
+      <c r="K32" s="4">
         <v>0.23</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="4" t="s">
-        <v>69</v>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
+        <v>1202</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C33" s="2">
         <v>12</v>
@@ -2016,16 +1892,16 @@
       <c r="J33" s="3">
         <v>0.75</v>
       </c>
-      <c r="K33" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="4" t="s">
-        <v>71</v>
+      <c r="K33" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="8">
+        <v>1203</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2">
         <v>12</v>
@@ -2051,16 +1927,16 @@
       <c r="J34" s="3">
         <v>0.23</v>
       </c>
-      <c r="K34" s="5">
+      <c r="K34" s="4">
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="4" t="s">
-        <v>73</v>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="8">
+        <v>1204</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="C35" s="2">
         <v>12</v>
@@ -2086,16 +1962,16 @@
       <c r="J35" s="3">
         <v>0.34</v>
       </c>
-      <c r="K35" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="25.5">
-      <c r="A36" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>76</v>
+      <c r="K35" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="8">
+        <v>1301</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="C36" s="2">
         <v>13</v>
@@ -2121,16 +1997,16 @@
       <c r="J36" s="3">
         <v>0.7</v>
       </c>
-      <c r="K36" s="5">
+      <c r="K36" s="4">
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="25.5">
-      <c r="A37" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>78</v>
+    <row r="37" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
+        <v>1401</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C37" s="2">
         <v>14</v>
@@ -2156,16 +2032,16 @@
       <c r="J37" s="3">
         <v>0.3</v>
       </c>
-      <c r="K37" s="5">
+      <c r="K37" s="4">
         <v>0.09</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="25.5">
-      <c r="A38" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>80</v>
+    <row r="38" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
+        <v>1501</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C38" s="2">
         <v>15</v>
@@ -2191,16 +2067,16 @@
       <c r="J38" s="3">
         <v>1</v>
       </c>
-      <c r="K38" s="5">
+      <c r="K38" s="4">
         <v>0.23</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="25.5">
-      <c r="A39" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>82</v>
+    <row r="39" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
+        <v>1601</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C39" s="2">
         <v>16</v>
@@ -2226,16 +2102,16 @@
       <c r="J39" s="3">
         <v>0.05</v>
       </c>
-      <c r="K39" s="5">
+      <c r="K39" s="4">
         <v>0.04</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="4" t="s">
-        <v>83</v>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="8">
+        <v>1701</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C40" s="2">
         <v>17</v>
@@ -2261,16 +2137,16 @@
       <c r="J40" s="3">
         <v>0.5</v>
       </c>
-      <c r="K40" s="5">
+      <c r="K40" s="4">
         <v>0.24</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="4" t="s">
-        <v>85</v>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
+        <v>1702</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C41" s="2">
         <v>17</v>
@@ -2296,16 +2172,16 @@
       <c r="J41" s="3">
         <v>0.05</v>
       </c>
-      <c r="K41" s="5">
+      <c r="K41" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="4" t="s">
-        <v>87</v>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="8">
+        <v>1703</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="C42" s="2">
         <v>17</v>
@@ -2331,16 +2207,16 @@
       <c r="J42" s="3">
         <v>0.1</v>
       </c>
-      <c r="K42" s="5">
+      <c r="K42" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="4" t="s">
-        <v>89</v>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
+        <v>1704</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C43" s="2">
         <v>17</v>
@@ -2366,16 +2242,16 @@
       <c r="J43" s="3">
         <v>0.05</v>
       </c>
-      <c r="K43" s="5">
+      <c r="K43" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="38.25">
-      <c r="A44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>92</v>
+    <row r="44" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="8">
+        <v>1801</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C44" s="2">
         <v>18</v>
@@ -2401,16 +2277,16 @@
       <c r="J44" s="3">
         <v>0.1</v>
       </c>
-      <c r="K44" s="5">
+      <c r="K44" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="25.5">
-      <c r="A45" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>94</v>
+    <row r="45" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="8">
+        <v>1901</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="C45" s="2">
         <v>19</v>
@@ -2436,16 +2312,16 @@
       <c r="J45" s="3">
         <v>0.1</v>
       </c>
-      <c r="K45" s="5">
+      <c r="K45" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="25.5">
-      <c r="A46" s="4" t="s">
-        <v>95</v>
+    <row r="46" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="8">
+        <v>2001</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="C46" s="2">
         <v>20</v>
@@ -2471,16 +2347,16 @@
       <c r="J46" s="3">
         <v>0.01</v>
       </c>
-      <c r="K46" s="5">
+      <c r="K46" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="25.5">
-      <c r="A47" s="4" t="s">
-        <v>97</v>
+    <row r="47" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="8">
+        <v>2002</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="C47" s="2">
         <v>20</v>
@@ -2506,16 +2382,16 @@
       <c r="J47" s="3">
         <v>0.01</v>
       </c>
-      <c r="K47" s="5">
+      <c r="K47" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="25.5">
-      <c r="A48" s="4" t="s">
-        <v>99</v>
+    <row r="48" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="8">
+        <v>2003</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="C48" s="2">
         <v>20</v>
@@ -2541,16 +2417,16 @@
       <c r="J48" s="3">
         <v>0.01</v>
       </c>
-      <c r="K48" s="5">
+      <c r="K48" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="4" t="s">
-        <v>101</v>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="8">
+        <v>2004</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="C49" s="2">
         <v>20</v>
@@ -2576,16 +2452,16 @@
       <c r="J49" s="3">
         <v>0.01</v>
       </c>
-      <c r="K49" s="5">
+      <c r="K49" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="51">
-      <c r="A50" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>104</v>
+    <row r="50" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A50" s="8">
+        <v>2101</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C50" s="2">
         <v>21</v>
@@ -2611,16 +2487,16 @@
       <c r="J50" s="3">
         <v>0.01</v>
       </c>
-      <c r="K50" s="5">
+      <c r="K50" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="25.5">
-      <c r="A51" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>106</v>
+    <row r="51" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="8">
+        <v>2201</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C51" s="2">
         <v>22</v>
@@ -2646,16 +2522,16 @@
       <c r="J51" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K51" s="5">
+      <c r="K51" s="4">
         <v>0.22</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="25.5">
-      <c r="A52" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>108</v>
+    <row r="52" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="8">
+        <v>2301</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C52" s="2">
         <v>23</v>
@@ -2681,16 +2557,16 @@
       <c r="J52" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K52" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="25.5">
-      <c r="A53" s="4" t="s">
-        <v>109</v>
+      <c r="K52" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A53" s="8">
+        <v>2401</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="C53" s="2">
         <v>24</v>
@@ -2716,16 +2592,16 @@
       <c r="J53" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K53" s="5">
+      <c r="K53" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="25.5">
-      <c r="A54" s="4" t="s">
-        <v>110</v>
+    <row r="54" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="8">
+        <v>2402</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="C54" s="2">
         <v>24</v>
@@ -2751,16 +2627,16 @@
       <c r="J54" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K54" s="5">
+      <c r="K54" s="4">
         <v>0.08</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="25.5">
-      <c r="A55" s="4" t="s">
-        <v>111</v>
+    <row r="55" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="8">
+        <v>2403</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="C55" s="2">
         <v>24</v>
@@ -2786,16 +2662,16 @@
       <c r="J55" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K55" s="5">
+      <c r="K55" s="4">
         <v>0.13</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="4" t="s">
-        <v>112</v>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="8">
+        <v>2404</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="C56" s="2">
         <v>24</v>
@@ -2821,16 +2697,16 @@
       <c r="J56" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K56" s="5">
+      <c r="K56" s="4">
         <v>0.12</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="51">
-      <c r="A57" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>114</v>
+    <row r="57" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A57" s="8">
+        <v>2501</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C57" s="2">
         <v>25</v>
@@ -2856,16 +2732,16 @@
       <c r="J57" s="3">
         <v>1E-3</v>
       </c>
-      <c r="K57" s="5">
+      <c r="K57" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>116</v>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="8">
+        <v>2601</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C58" s="2">
         <v>26</v>
@@ -2891,16 +2767,16 @@
       <c r="J58" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K58" s="5">
+      <c r="K58" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="25.5">
-      <c r="A59" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>118</v>
+    <row r="59" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="8">
+        <v>2701</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C59" s="2">
         <v>27</v>
@@ -2926,11 +2802,47 @@
       <c r="J59" s="3">
         <v>0.01</v>
       </c>
-      <c r="K59" s="5">
+      <c r="K59" s="4">
         <v>0.08</v>
       </c>
     </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="8">
+        <v>2801</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="11">
+        <v>28</v>
+      </c>
+      <c r="D60" s="12">
+        <v>0</v>
+      </c>
+      <c r="E60" s="12">
+        <v>0</v>
+      </c>
+      <c r="F60" s="12">
+        <v>0</v>
+      </c>
+      <c r="G60" s="12">
+        <v>0</v>
+      </c>
+      <c r="H60" s="12">
+        <v>0</v>
+      </c>
+      <c r="I60" s="12">
+        <v>0</v>
+      </c>
+      <c r="J60" s="13">
+        <v>0</v>
+      </c>
+      <c r="K60" s="14">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>